<commit_message>
msz - floProfil first tc is running
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgBaseNormal.xlsx
+++ b/Data/Dialogs/dlgBaseNormal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF88B65B-7CDA-40E0-AC9E-B3B45817C395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7789F4-A405-4B91-B4D6-B174822CB3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1980" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="40440" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -640,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
msz - second reset-pwd-testcase + control updates
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgBaseNormal.xlsx
+++ b/Data/Dialogs/dlgBaseNormal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1122982-221F-49F6-9953-83EC229BE484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F324B9-9221-4C86-8011-22F574964A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6012" yWindow="1380" windowWidth="31284" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="492" yWindow="300" windowWidth="40212" windowHeight="14580" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
   <si>
     <t>Action</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Menueauswahl Mein Profil</t>
   </si>
   <si>
-    <t>menUeberblick</t>
-  </si>
-  <si>
     <t>menChat</t>
   </si>
   <si>
@@ -249,7 +246,79 @@
     <t>Mobile</t>
   </si>
   <si>
-    <t>//android.widget.TextView[@text=""]</t>
+    <t>menUebersicht</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Übersicht"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Chat 0"]</t>
+  </si>
+  <si>
+    <t>xpath=</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Meine Termine"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Mein Profil"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Meine Spiele"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Mein Verein"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Mobile App"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Mitglieder"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Trainings"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Mannschaften"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Spieltermine"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Vereinstermine"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Verein"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Orte &amp; Schlüssel"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.view.View[@content-desc=" Umfragen"]</t>
+  </si>
+  <si>
+    <t>xpath=(//android.widget.ListView/android.view.View/android.view.View[@content-desc=" Abwesenheiten"])</t>
+  </si>
+  <si>
+    <t>xpath=////android.view.View[@content-desc="logo"]</t>
+  </si>
+  <si>
+    <t>//android.view.View[@content-desc=""]</t>
+  </si>
+  <si>
+    <t>butCollapseMenu</t>
+  </si>
+  <si>
+    <t>butNotifications</t>
+  </si>
+  <si>
+    <t>xpath=//android.widget.Button[@text=" aktiv"]</t>
+  </si>
+  <si>
+    <t>xpath=//android.webkit.WebView/android.view.View[1]/android.view.View3]/android.widget.ListView/android.view.View[2]//android.widget.TextView</t>
+  </si>
+  <si>
+    <t>xpath=//android.webkit.WebView/android.view.View[1]/android.view.View3]/android.widget.ListView/android.view.View[3]//android.widget.TextView</t>
   </si>
 </sst>
 </file>
@@ -273,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +361,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -305,11 +386,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -337,8 +420,8 @@
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>624629</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3238289</xdr:colOff>
       <xdr:row>89</xdr:row>
       <xdr:rowOff>156587</xdr:rowOff>
     </xdr:to>
@@ -673,135 +756,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.21875" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" customWidth="1"/>
-    <col min="8" max="20" width="18.44140625" customWidth="1"/>
-    <col min="21" max="21" width="21.6640625" customWidth="1"/>
-    <col min="23" max="23" width="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13" customWidth="1"/>
-    <col min="25" max="25" width="42.5546875" customWidth="1"/>
+    <col min="3" max="3" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1"/>
+    <col min="5" max="5" width="54" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="58.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="56" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="54.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="58" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="58.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="61.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="92.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" customWidth="1"/>
+    <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="43.109375" customWidth="1"/>
+    <col min="27" max="27" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>36</v>
-      </c>
+      <c r="D1" s="5"/>
       <c r="E1" t="s">
         <v>35</v>
       </c>
       <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>44</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>46</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>48</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>49</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="AA1" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="F2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -810,76 +961,82 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="T3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -889,10 +1046,7 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="V4" t="s">
@@ -904,30 +1058,33 @@
       <c r="X4" t="s">
         <v>15</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>15</v>
       </c>
-      <c r="Z4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="Y5" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -935,245 +1092,245 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="Z6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AB6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>54</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>55</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>57</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>58</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>59</v>
       </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="M16" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>60</v>
       </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="N17" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="P18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
-        <v>12</v>
-      </c>
-      <c r="O18" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>62</v>
       </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="P19" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="R20" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>63</v>
       </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="S21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>64</v>
       </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="R21" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="T22" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>65</v>
       </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="S22" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="T23" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z23" t="s">
+      <c r="U23" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB23" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
msz - more control updates + experiments
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgBaseNormal.xlsx
+++ b/Data/Dialogs/dlgBaseNormal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F324B9-9221-4C86-8011-22F574964A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585D9C42-C77D-4B78-9050-68044FE28E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="492" yWindow="300" windowWidth="40212" windowHeight="14580" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="8052" yWindow="288" windowWidth="26088" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
msz - meinprofil.allgemein.check defaults ok
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgBaseNormal.xlsx
+++ b/Data/Dialogs/dlgBaseNormal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585D9C42-C77D-4B78-9050-68044FE28E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C0B6D3-DD73-4D51-AE50-604BCA491BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8052" yWindow="288" windowWidth="26088" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="1020" yWindow="516" windowWidth="38676" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -318,7 +318,7 @@
     <t>xpath=//android.webkit.WebView/android.view.View[1]/android.view.View3]/android.widget.ListView/android.view.View[2]//android.widget.TextView</t>
   </si>
   <si>
-    <t>xpath=//android.webkit.WebView/android.view.View[1]/android.view.View3]/android.widget.ListView/android.view.View[3]//android.widget.TextView</t>
+    <t>xpath=(//android.view.View[@resource-id="navbar-collapse"])[2]/android.widget.ListView/android.view.View[3]/android.view.View/android.widget.TextView</t>
   </si>
 </sst>
 </file>
@@ -758,8 +758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82737E07-8287-4E6B-9130-6C87B574EFB8}">
   <dimension ref="A1:AB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,6 +1336,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
msz - starting table control and integrate the record reader within
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgBaseNormal.xlsx
+++ b/Data/Dialogs/dlgBaseNormal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C0B6D3-DD73-4D51-AE50-604BCA491BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F179704-CC52-4286-8464-5A27B9B1704E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="516" windowWidth="38676" windowHeight="15300" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="4824" yWindow="2016" windowWidth="33996" windowHeight="13668" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -759,7 +759,7 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,7 +788,7 @@
     <col min="22" max="22" width="21.6640625" customWidth="1"/>
     <col min="24" max="24" width="13" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="43.109375" customWidth="1"/>
+    <col min="26" max="26" width="48.5546875" customWidth="1"/>
     <col min="27" max="27" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
msz - replacing AppiumLibrary by native python-appium-client (part 2)
</commit_message>
<xml_diff>
--- a/Data/Dialogs/dlgBaseNormal.xlsx
+++ b/Data/Dialogs/dlgBaseNormal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\OnTop\Data\Dialogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F179704-CC52-4286-8464-5A27B9B1704E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FF7A21-234F-48AC-8AB1-0DB9243B49BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4824" yWindow="2016" windowWidth="33996" windowHeight="13668" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
+    <workbookView xWindow="3444" yWindow="1248" windowWidth="35136" windowHeight="13680" xr2:uid="{AE079285-A10A-4E50-89E0-1FC0BD4174C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -318,7 +318,7 @@
     <t>xpath=//android.webkit.WebView/android.view.View[1]/android.view.View3]/android.widget.ListView/android.view.View[2]//android.widget.TextView</t>
   </si>
   <si>
-    <t>xpath=(//android.view.View[@resource-id="navbar-collapse"])[2]/android.widget.ListView/android.view.View[3]/android.view.View/android.widget.TextView</t>
+    <t>xpath=//android.view.View[@resource-id='navbar-collapse'][2]/android.widget.ListView/android.view.View[3]/android.view.View/android.widget.TextView</t>
   </si>
 </sst>
 </file>
@@ -759,7 +759,7 @@
   <dimension ref="A1:AB23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>